<commit_message>
Versao Final UiPath Teste
</commit_message>
<xml_diff>
--- a/WorkItems.xlsx
+++ b/WorkItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb1daaaab9671875/Documentos/UiPath/Teste_Robo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{26844625-88C5-4125-B447-9C23A24AA216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04DBA36C-BE51-4EFA-BFD8-1CF9D50BACE5}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{26844625-88C5-4125-B447-9C23A24AA216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CAD3948-8059-4306-B6E8-A185500A10F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8FA25497-F4B3-4C53-9A38-A8108D53950D}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="E2:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D18" sqref="A1:E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>